<commit_message>
go audio creater added
</commit_message>
<xml_diff>
--- a/French.xlsx
+++ b/French.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="249">
   <si>
     <t>salut</t>
   </si>
@@ -577,6 +577,195 @@
   </si>
   <si>
     <t>c'est quelque chose de difficile? non, mais c'est très necessaire de le faire maintenant</t>
+  </si>
+  <si>
+    <t>Clase 3</t>
+  </si>
+  <si>
+    <t>necesito hacerlo</t>
+  </si>
+  <si>
+    <t>j'ai besoin de le faire</t>
+  </si>
+  <si>
+    <t>no necesito hacerlo</t>
+  </si>
+  <si>
+    <t>je n'ai pas besoin de le faire</t>
+  </si>
+  <si>
+    <t>necesito estar aquí</t>
+  </si>
+  <si>
+    <t>j'ai besoin d'être ici</t>
+  </si>
+  <si>
+    <t>no necesito estar aquí</t>
+  </si>
+  <si>
+    <t>je n'ai pas besoin d'être ici</t>
+  </si>
+  <si>
+    <t>no necesito estar aquí hoy</t>
+  </si>
+  <si>
+    <t>je n'ai pas besoin d'être ici aujourd'hui</t>
+  </si>
+  <si>
+    <t>necesito hacerlo ahora</t>
+  </si>
+  <si>
+    <t>j'ai besoin d'être maintenant</t>
+  </si>
+  <si>
+    <t>necesito estar aquí ahora</t>
+  </si>
+  <si>
+    <t>j'ai besoin d'être ici maintenant</t>
+  </si>
+  <si>
+    <t>porque</t>
+  </si>
+  <si>
+    <t>parce que</t>
+  </si>
+  <si>
+    <t>porque es importante</t>
+  </si>
+  <si>
+    <t>parce que c'est très important</t>
+  </si>
+  <si>
+    <t>necesito hacerlo hoy porque es importante</t>
+  </si>
+  <si>
+    <t>j'ai besoin de le faire aujourd'hui parce que c'est important</t>
+  </si>
+  <si>
+    <t>necesito estar aquí hoy porque es importante</t>
+  </si>
+  <si>
+    <t>j'ai besoin d'être ici aujourd'hui parce que c'est important</t>
+  </si>
+  <si>
+    <t>es posible</t>
+  </si>
+  <si>
+    <t>c'est possible</t>
+  </si>
+  <si>
+    <t>no es posible</t>
+  </si>
+  <si>
+    <t>ce n'est pas possible</t>
+  </si>
+  <si>
+    <t>ahora, no es posible</t>
+  </si>
+  <si>
+    <t>maintenant, ce n'est pas possible</t>
+  </si>
+  <si>
+    <t>saber</t>
+  </si>
+  <si>
+    <t>savoir</t>
+  </si>
+  <si>
+    <t>necesito saber</t>
+  </si>
+  <si>
+    <t>j'ai besoin de savoir</t>
+  </si>
+  <si>
+    <t>si (condicional)</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>sí (afirmacion)</t>
+  </si>
+  <si>
+    <t>si es posible</t>
+  </si>
+  <si>
+    <t>si c'est possible</t>
+  </si>
+  <si>
+    <t>si es posible para mi</t>
+  </si>
+  <si>
+    <t>si c'est possible pour moi</t>
+  </si>
+  <si>
+    <t>necesito saber si es posible</t>
+  </si>
+  <si>
+    <t>j'ai besoin de savoir si c'est possible</t>
+  </si>
+  <si>
+    <t>necesito saber si es posible hoy</t>
+  </si>
+  <si>
+    <t>j'ai besoin de savoir si c'est possible aujourd'hui</t>
+  </si>
+  <si>
+    <t>necesito saber si es posible hacerlo hoy</t>
+  </si>
+  <si>
+    <t>j'ai besoin de savoir si c'est possible de le faire aujourd'hui</t>
+  </si>
+  <si>
+    <t>necesito saber si es posible hacerlo ahora porque es muy importante</t>
+  </si>
+  <si>
+    <t>j'ai besoin de savoir si c'est possible de le faire maintenant parce que c'est très important</t>
+  </si>
+  <si>
+    <t>necesito saber si es algo importante</t>
+  </si>
+  <si>
+    <t>j'ai besoin de savoir si c'est quelque chose d'important</t>
+  </si>
+  <si>
+    <t>yo quiero</t>
+  </si>
+  <si>
+    <t>je veux</t>
+  </si>
+  <si>
+    <t>quiero hacerlo</t>
+  </si>
+  <si>
+    <t>je veux le faire</t>
+  </si>
+  <si>
+    <t>quiero hacerlo hoy</t>
+  </si>
+  <si>
+    <t>je veux le faire aujourd'hui</t>
+  </si>
+  <si>
+    <t>no quiero</t>
+  </si>
+  <si>
+    <t>je ne veux pas</t>
+  </si>
+  <si>
+    <t>no quiero hacerlo así</t>
+  </si>
+  <si>
+    <t>je ne veux pas le faire comme ça</t>
+  </si>
+  <si>
+    <t>quiero saber si es fácil para mí hacerlo hoy</t>
+  </si>
+  <si>
+    <t>je veux savoir si c'est facile pour moi de le faire aujourd'hui</t>
   </si>
 </sst>
 </file>
@@ -894,13 +1083,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1641,6 +1834,259 @@
       </c>
       <c r="B90" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>187</v>
+      </c>
+      <c r="B92" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>189</v>
+      </c>
+      <c r="B93" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>191</v>
+      </c>
+      <c r="B94" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>193</v>
+      </c>
+      <c r="B95" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>195</v>
+      </c>
+      <c r="B96" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>197</v>
+      </c>
+      <c r="B97" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>199</v>
+      </c>
+      <c r="B98" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>203</v>
+      </c>
+      <c r="B100" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>205</v>
+      </c>
+      <c r="B101" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>207</v>
+      </c>
+      <c r="B102" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>209</v>
+      </c>
+      <c r="B103" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>211</v>
+      </c>
+      <c r="B104" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>213</v>
+      </c>
+      <c r="B105" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>215</v>
+      </c>
+      <c r="B106" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>217</v>
+      </c>
+      <c r="B107" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>219</v>
+      </c>
+      <c r="B108" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>222</v>
+      </c>
+      <c r="B109" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>223</v>
+      </c>
+      <c r="B110" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>225</v>
+      </c>
+      <c r="B111" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>227</v>
+      </c>
+      <c r="B112" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>229</v>
+      </c>
+      <c r="B113" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>231</v>
+      </c>
+      <c r="B114" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>233</v>
+      </c>
+      <c r="B115" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>235</v>
+      </c>
+      <c r="B116" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>237</v>
+      </c>
+      <c r="B117" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>239</v>
+      </c>
+      <c r="B118" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>241</v>
+      </c>
+      <c r="B119" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>243</v>
+      </c>
+      <c r="B120" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>245</v>
+      </c>
+      <c r="B121" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>247</v>
+      </c>
+      <c r="B122" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>